<commit_message>
BOM and gerber with changed connector
</commit_message>
<xml_diff>
--- a/hardware/Scrutineering/BOM/Scrutineering.xlsx
+++ b/hardware/Scrutineering/BOM/Scrutineering.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phoen\LHR\PS-VoltTemp\hardware\Scrutineering\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DB0C0C-66EA-407D-80B4-7F2AC9E5A7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231F4224-F0DA-4BEB-A467-4C0461C5263A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="10" windowWidth="25820" windowHeight="16220" xr2:uid="{62597573-C5BD-43BE-8C8F-E66FE9158839}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{62597573-C5BD-43BE-8C8F-E66FE9158839}"/>
   </bookViews>
   <sheets>
     <sheet name="Scrutineering" sheetId="1" r:id="rId1"/>
@@ -25,24 +25,15 @@
     <t>Reference</t>
   </si>
   <si>
-    <t>J1,J2,J3,J4</t>
-  </si>
-  <si>
     <t>Value</t>
   </si>
   <si>
-    <t>Conn_01x04</t>
-  </si>
-  <si>
     <t>P/N</t>
   </si>
   <si>
     <t>Footprint</t>
   </si>
   <si>
-    <t>VoltTemp:1053132104</t>
-  </si>
-  <si>
     <t>Qty</t>
   </si>
   <si>
@@ -55,18 +46,12 @@
     <t>UTSVT_Connectors:Banana_Jack_1_Pin_4mm</t>
   </si>
   <si>
-    <t>J11,J12</t>
-  </si>
-  <si>
     <t>Conn_01x03</t>
   </si>
   <si>
     <t>VoltTemp:1053131103</t>
   </si>
   <si>
-    <t>J13,J14</t>
-  </si>
-  <si>
     <t>Conn_01x02</t>
   </si>
   <si>
@@ -86,6 +71,21 @@
   </si>
   <si>
     <t>105-2210-201</t>
+  </si>
+  <si>
+    <t>J1,J2</t>
+  </si>
+  <si>
+    <t>Conn_02x04</t>
+  </si>
+  <si>
+    <t>Scrutineering:nanofit_02x04</t>
+  </si>
+  <si>
+    <t>J3,J4</t>
+  </si>
+  <si>
+    <t>J11,J11</t>
   </si>
 </sst>
 </file>
@@ -949,120 +949,122 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.08984375" customWidth="1"/>
-    <col min="2" max="2" width="13.90625" customWidth="1"/>
-    <col min="3" max="3" width="12.1796875" customWidth="1"/>
-    <col min="4" max="4" width="12.08984375" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2">
-        <v>1053132104</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>4</v>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>1053132102</v>
+      </c>
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
       </c>
       <c r="C4">
         <v>1053131103</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>1053132102</v>
+        <v>1053141108</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E11">
+    <sortCondition ref="B1:B11"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>